<commit_message>
Programming Basics - Jan 2016 - Lecture_01. First Steps in Coding + Tasks
</commit_message>
<xml_diff>
--- a/Programming Basics - Jan 2016/Programming-Basics-Course-Program-Jan-2015.xlsx
+++ b/Programming Basics - Jan 2016/Programming-Basics-Course-Program-Jan-2015.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="9735" tabRatio="245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="9750" tabRatio="245"/>
   </bookViews>
   <sheets>
     <sheet name="Programming Basics" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="74">
   <si>
     <t>Content</t>
   </si>
@@ -233,16 +233,16 @@
   </si>
   <si>
     <t>Четене и печатане на числа, променливи, прости сметки</t>
+  </si>
+  <si>
+    <t>16:00-20:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\-mmm"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,14 +263,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -326,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -370,14 +362,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -395,16 +386,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1028,32 +1016,32 @@
     <col min="2" max="2" width="32.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="85.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1093,7 +1081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -1133,7 +1121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -1175,7 +1163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -1218,7 +1206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -1261,7 +1249,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -1304,7 +1292,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>4</v>
       </c>
@@ -1347,11 +1335,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1390,11 +1378,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1437,7 +1425,7 @@
       <c r="A11" s="6">
         <v>7</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="12" t="s">
@@ -1476,9 +1464,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -1514,7 +1502,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>8</v>
       </c>
@@ -1528,14 +1516,14 @@
         <v>5</v>
       </c>
       <c r="E13" s="3">
-        <v>42434</v>
+        <v>42435</v>
       </c>
       <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Saturday</v>
+        <v>Sunday</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>4</v>
@@ -1544,40 +1532,40 @@
         <v>5</v>
       </c>
       <c r="J13" s="3">
-        <v>42434</v>
+        <v>42435</v>
       </c>
       <c r="K13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>Saturday</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>23</v>
+        <v>Sunday</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="14" t="s">
@@ -1601,14 +1589,14 @@
       <c r="J15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="18" t="s">
+      <c r="L15" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>0</v>
       </c>
@@ -1648,7 +1636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>1</v>
       </c>
@@ -1691,7 +1679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>1</v>
       </c>
@@ -1734,7 +1722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>2</v>
       </c>
@@ -1777,7 +1765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>2</v>
       </c>
@@ -1820,7 +1808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>3</v>
       </c>
@@ -1834,7 +1822,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" ref="E21:E26" si="4">E20+7</f>
+        <f t="shared" ref="E21:E22" si="4">E20+7</f>
         <v>42454</v>
       </c>
       <c r="F21" s="3" t="str">
@@ -1863,7 +1851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>4</v>
       </c>
@@ -1906,7 +1894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>4</v>
       </c>
@@ -1949,78 +1937,78 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>5</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="3">
+        <f>E23+7</f>
+        <v>42468</v>
+      </c>
+      <c r="F24" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>Friday</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="9">
+        <f>Table132[[#This Row],[Date]]+7</f>
+        <v>42475</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="3">
-        <v>42463</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="24" t="s">
+      <c r="J24" s="3">
+        <f>J22+7</f>
+        <v>42469</v>
+      </c>
+      <c r="K24" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Saturday</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>6</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3">
-        <f>E23+7</f>
-        <v>42468</v>
-      </c>
-      <c r="F25" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>Friday</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="9">
-        <f>Table132[[#This Row],[Date]]+7</f>
-        <v>42475</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J25" s="3">
-        <f>J22+7</f>
-        <v>42469</v>
-      </c>
-      <c r="K25" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Saturday</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>42470</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>7</v>
       </c>
@@ -2034,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="4"/>
+        <f>E24+7</f>
         <v>42475</v>
       </c>
       <c r="F26" s="3" t="str">
@@ -2052,7 +2040,7 @@
         <v>31</v>
       </c>
       <c r="J26" s="3">
-        <f>J25+7</f>
+        <f>J24+7</f>
         <v>42476</v>
       </c>
       <c r="K26" s="3" t="str">
@@ -2082,7 +2070,7 @@
       <c r="F27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="18" t="s">
         <v>55</v>
       </c>
       <c r="H27" s="5" t="s">
@@ -2097,7 +2085,7 @@
       <c r="K27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L27" s="19" t="s">
+      <c r="L27" s="18" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2112,14 +2100,14 @@
       <c r="D28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="H28" s="21" t="s">
+      <c r="E28" s="19"/>
+      <c r="H28" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="23"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>